<commit_message>
moved homebrew to direct source
</commit_message>
<xml_diff>
--- a/source-gen.xlsx
+++ b/source-gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tagge\Documents\GitHub\BraveYearbook.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D18CF23-A74E-423C-B893-1A8F903BF66F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D3D68E-6600-4ECF-A13B-A39EE604CFBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10208" xr2:uid="{86890A33-AE11-41B0-9A17-3F609C963544}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Index</t>
   </si>
@@ -43,51 +43,6 @@
     <t>DM</t>
   </si>
   <si>
-    <t>DM2</t>
-  </si>
-  <si>
-    <t>DM3</t>
-  </si>
-  <si>
-    <t>DM4</t>
-  </si>
-  <si>
-    <t>DM5</t>
-  </si>
-  <si>
-    <t>DM6</t>
-  </si>
-  <si>
-    <t>DM7</t>
-  </si>
-  <si>
-    <t>DM8</t>
-  </si>
-  <si>
-    <t>DM9</t>
-  </si>
-  <si>
-    <t>DM10</t>
-  </si>
-  <si>
-    <t>DM11</t>
-  </si>
-  <si>
-    <t>DM12</t>
-  </si>
-  <si>
-    <t>DM13</t>
-  </si>
-  <si>
-    <t>DM14</t>
-  </si>
-  <si>
-    <t>DM15</t>
-  </si>
-  <si>
-    <t>DM16</t>
-  </si>
-  <si>
     <t>Json to Full</t>
   </si>
   <si>
@@ -97,9 +52,6 @@
     <t>Var</t>
   </si>
   <si>
-    <t>AM1</t>
-  </si>
-  <si>
     <t>KCAA</t>
   </si>
   <si>
@@ -130,9 +82,6 @@
     <t>Acute Magic</t>
   </si>
   <si>
-    <t>Lexi</t>
-  </si>
-  <si>
     <t>Clockwork Magic</t>
   </si>
   <si>
@@ -185,12 +134,24 @@
   </si>
   <si>
     <t>Everyday Rituals for the Travelling Wizard</t>
+  </si>
+  <si>
+    <t>Words of the Lexi</t>
+  </si>
+  <si>
+    <t>Book of Lost Spells</t>
+  </si>
+  <si>
+    <t>BoLS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,8 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,49 +499,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADE2215-93D6-44D2-95F6-83C55A62FA7B}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L21"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="3" max="3" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="9.06640625" style="2"/>
     <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="61.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -586,37 +552,37 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="str">
-        <f>A2&amp;C2</f>
-        <v>DM1</v>
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>A2&amp;TEXT(C2,"00")</f>
+        <v>DM01</v>
       </c>
       <c r="F2" t="str">
-        <f>B2&amp; " " &amp;C2 &amp; ": " &amp; D2</f>
-        <v>Deep Magic 1: Clockwork Magic</v>
+        <f>B2&amp; " " &amp;TEXT(C2,"00") &amp; ": " &amp; D2</f>
+        <v>Deep Magic 01: Clockwork Magic</v>
       </c>
       <c r="I2" t="str">
         <f>"SRC_HB"&amp;E2</f>
-        <v>SRC_HBDM1</v>
+        <v>SRC_HBDM01</v>
       </c>
       <c r="J2" t="str">
         <f>I2 &amp; " = SRC_HB_PREFIX + """ &amp; E2 &amp; """;"</f>
-        <v>SRC_HBDM1 = SRC_HB_PREFIX + "DM1";</v>
+        <v>SRC_HBDM01 = SRC_HB_PREFIX + "DM01";</v>
       </c>
       <c r="K2" t="str">
         <f>"Parser.SOURCE_JSON_TO_FULL["&amp;I2&amp;"] = """ &amp; F2 &amp; """;"</f>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM1] = "Deep Magic 1: Clockwork Magic";</v>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM01] = "Deep Magic 01: Clockwork Magic";</v>
       </c>
       <c r="L2" t="str">
-        <f>"Parser.SOURCE_JSON_TO_ABV["&amp;I2&amp;"] = ""HB" &amp; E2 &amp;""";"</f>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM1] = "HBDM1";</v>
+        <f>"Parser.SOURCE_JSON_TO_ABV["&amp;I2&amp;"] = """ &amp; E2 &amp;""";"</f>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM01] = "DM01";</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -624,36 +590,37 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f t="shared" ref="E3:E21" si="0">A3&amp;TEXT(C3,"00")</f>
+        <v>DM02</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F18" si="0">B3&amp; " " &amp;C3 &amp; ": " &amp; D3</f>
-        <v>Deep Magic 2: Rune Magic</v>
+        <f t="shared" ref="F3:F18" si="1">B3&amp; " " &amp;TEXT(C3,"00") &amp; ": " &amp; D3</f>
+        <v>Deep Magic 02: Rune Magic</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="1">"SRC_HB"&amp;E3</f>
-        <v>SRC_HBDM2</v>
+        <f t="shared" ref="I3:I22" si="2">"SRC_HB"&amp;E3</f>
+        <v>SRC_HBDM02</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="2">I3 &amp; " = SRC_HB_PREFIX + """ &amp; E3 &amp; """;"</f>
-        <v>SRC_HBDM2 = SRC_HB_PREFIX + "DM2";</v>
+        <f t="shared" ref="J3:J22" si="3">I3 &amp; " = SRC_HB_PREFIX + """ &amp; E3 &amp; """;"</f>
+        <v>SRC_HBDM02 = SRC_HB_PREFIX + "DM02";</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="3">"Parser.SOURCE_JSON_TO_FULL["&amp;I3&amp;"] = """ &amp; F3 &amp; """;"</f>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM2] = "Deep Magic 2: Rune Magic";</v>
+        <f t="shared" ref="K3:K22" si="4">"Parser.SOURCE_JSON_TO_FULL["&amp;I3&amp;"] = """ &amp; F3 &amp; """;"</f>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM02] = "Deep Magic 02: Rune Magic";</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L21" si="4">"Parser.SOURCE_JSON_TO_ABV["&amp;I3&amp;"] = ""HB" &amp; E3 &amp;""";"</f>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM2] = "HBDM2";</v>
+        <f t="shared" ref="L3:L22" si="5">"Parser.SOURCE_JSON_TO_ABV["&amp;I3&amp;"] = """ &amp; E3 &amp;""";"</f>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM02] = "DM02";</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -661,36 +628,37 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM03</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 3: Void Magic</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 03: Void Magic</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM3</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM03</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM3 = SRC_HB_PREFIX + "DM3";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM03 = SRC_HB_PREFIX + "DM03";</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM3] = "Deep Magic 3: Void Magic";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM03] = "Deep Magic 03: Void Magic";</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM3] = "HBDM3";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM03] = "DM03";</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -698,36 +666,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM04</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 4: Illumination Magic</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 04: Illumination Magic</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM4</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM04</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM4 = SRC_HB_PREFIX + "DM4";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM04 = SRC_HB_PREFIX + "DM04";</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM4] = "Deep Magic 4: Illumination Magic";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM04] = "Deep Magic 04: Illumination Magic";</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM4] = "HBDM4";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM04] = "DM04";</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -735,36 +704,37 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM05</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 5: Ley Lines</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 05: Ley Lines</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM5</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM05</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM5 = SRC_HB_PREFIX + "DM5";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM05 = SRC_HB_PREFIX + "DM05";</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM5] = "Deep Magic 5: Ley Lines";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM05] = "Deep Magic 05: Ley Lines";</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM5] = "HBDM5";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM05] = "DM05";</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -772,36 +742,37 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM06</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 6: Angelic Seals</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 06: Angelic Seals</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM6</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM06</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM6 = SRC_HB_PREFIX + "DM6";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM06 = SRC_HB_PREFIX + "DM06";</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM6] = "Deep Magic 6: Angelic Seals";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM06] = "Deep Magic 06: Angelic Seals";</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM6] = "HBDM6";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM06] = "DM06";</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -809,36 +780,37 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM07</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 7: Chaos Magic</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 07: Chaos Magic</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM7</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM07</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM7 = SRC_HB_PREFIX + "DM7";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM07 = SRC_HB_PREFIX + "DM07";</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM7] = "Deep Magic 7: Chaos Magic";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM07] = "Deep Magic 07: Chaos Magic";</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM7] = "HBDM7";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM07] = "DM07";</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -846,36 +818,37 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM08</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 8: Battle Magic</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 08: Battle Magic</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM8</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM08</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM8 = SRC_HB_PREFIX + "DM8";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM08 = SRC_HB_PREFIX + "DM08";</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM8] = "Deep Magic 8: Battle Magic";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM08] = "Deep Magic 08: Battle Magic";</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM8] = "HBDM8";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM08] = "DM08";</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -883,36 +856,37 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM09</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>Deep Magic 9: Ring Magic</v>
+        <f t="shared" si="1"/>
+        <v>Deep Magic 09: Ring Magic</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBDM9</v>
+        <f t="shared" si="2"/>
+        <v>SRC_HBDM09</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBDM9 = SRC_HB_PREFIX + "DM9";</v>
+        <f t="shared" si="3"/>
+        <v>SRC_HBDM09 = SRC_HB_PREFIX + "DM09";</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM9] = "Deep Magic 9: Ring Magic";</v>
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM09] = "Deep Magic 09: Ring Magic";</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM9] = "HBDM9";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM09] = "DM09";</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -920,36 +894,37 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM10</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 10: Shadow Magic</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM10</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM10 = SRC_HB_PREFIX + "DM10";</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM10] = "Deep Magic 10: Shadow Magic";</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM10] = "HBDM10";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM10] = "DM10";</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
@@ -957,36 +932,37 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM11</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 11: Elven High Magic</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM11</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM11 = SRC_HB_PREFIX + "DM11";</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM11] = "Deep Magic 11: Elven High Magic";</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM11] = "HBDM11";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM11] = "DM11";</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
@@ -994,36 +970,37 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM12</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 12: Blood &amp; Doom</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM12</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM12 = SRC_HB_PREFIX + "DM12";</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM12] = "Deep Magic 12: Blood &amp; Doom";</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM12] = "HBDM12";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM12] = "DM12";</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
@@ -1031,36 +1008,37 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
+      <c r="E14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM13</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 13: Dragon Magic</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM13</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM13 = SRC_HB_PREFIX + "DM13";</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM13] = "Deep Magic 13: Dragon Magic";</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM13] = "HBDM13";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM13] = "DM13";</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
@@ -1068,36 +1046,37 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="E15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM14</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 14: Elemental Magic</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM14</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM14 = SRC_HB_PREFIX + "DM14";</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM14] = "Deep Magic 14: Elemental Magic";</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM14] = "HBDM14";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM14] = "DM14";</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -1105,36 +1084,37 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="E16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM15</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 15: Hieroglyph Magic</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM15</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM15 = SRC_HB_PREFIX + "DM15";</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM15] = "Deep Magic 15: Hieroglyph Magic";</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM15] = "HBDM15";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM15] = "DM15";</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
@@ -1142,145 +1122,171 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="E17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>DM16</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Deep Magic 16: Time Magic</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBDM16</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBDM16 = SRC_HB_PREFIX + "DM16";</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBDM16] = "Deep Magic 16: Time Magic";</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM16] = "HBDM16";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBDM16] = "DM16";</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>AM01</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>Acute Magic 01: Words of the Lexi</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>SRC_HBAM01</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>SRC_HBAM01 = SRC_HB_PREFIX + "AM01";</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBAM01] = "Acute Magic 01: Words of the Lexi";</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBAM01] = "AM01";</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>SRC_HBKCAA</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>SRC_HBKCAA = SRC_HB_PREFIX + "KCAA";</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBKCAA] = "The Korranberg Chronicle: Adventurer's Almanac";</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBKCAA] = "KCAA";</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>SRC_HBFE</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>SRC_HBFE = SRC_HB_PREFIX + "FE";</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBFE] = "Faithful of Eberron";</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBFE] = "FE";</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>Acute Magic 1: Lexi</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBAM1</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBAM1 = SRC_HB_PREFIX + "AM1";</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBAM1] = "Acute Magic 1: Lexi";</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBAM1] = "HBAM1";</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBKCAA</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBKCAA = SRC_HB_PREFIX + "KCAA";</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBKCAA] = "The Korranberg Chronicle: Adventurer's Almanac";</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBKCAA] = "HBKCAA";</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>SRC_HBFE</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="2"/>
-        <v>SRC_HBFE = SRC_HB_PREFIX + "FE";</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="3"/>
-        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBFE] = "Faithful of Eberron";</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBFE] = "HBFE";</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SRC_HBERTW</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SRC_HBERTW = SRC_HB_PREFIX + "ERTW";</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBERTW] = "Everyday Rituals for the Travelling Wizard";</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="4"/>
-        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBERTW] = "HBERTW";</v>
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBERTW] = "ERTW";</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>SRC_HBBoLS</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>SRC_HBBoLS = SRC_HB_PREFIX + "BoLS";</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>Parser.SOURCE_JSON_TO_FULL[SRC_HBBoLS] = "Book of Lost Spells";</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>Parser.SOURCE_JSON_TO_ABV[SRC_HBBoLS] = "BoLS";</v>
       </c>
     </row>
   </sheetData>

</xml_diff>